<commit_message>
A KEY file is now generated in Metrics
Closes #20
</commit_message>
<xml_diff>
--- a/processing/test2/20230613-a1r-nc-session3-a_transcript.xlsx
+++ b/processing/test2/20230613-a1r-nc-session3-a_transcript.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,1542 +424,2669 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>speaker</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>time</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>text</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Has Arguments</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>All Arguments Summarized</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B2" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>"2:08"</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>It's the same group as it was last time, so I'm ace high.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
         <v>48653</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>"2:18"</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Can you guys hear me, okay?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B4" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>"10:22"</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>I can start. Hopefully, you can hear me, but I probably against allowing people to register to vote online. So in Montana, the forms to register to vote are online and you can pull it out as a PDF, but you still have to mail it in. I'm not a huge fan of allowing it to be registered online. I think it just opens it up to way too much fraud software, developer. And I know how easy it is to kind of just automate a lot of those forms. So,</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The text discusses the issue of online voter registration.
+2. The author is generally against allowing people to register to vote online.
+3. In Montana, forms for voter registration are available online as PDFs, but they still need to be mailed in.
+4. The author is not a fan of online registration due to the potential for fraud.
+5. The author is aware of the ease with which software can automate forms, implying that this could be used for fraudulent voter registrations.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B5" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>"10:22"</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t xml:space="preserve"> So I'm not a big fan of that. I am a fan though of allowing people to register up to and including the day of the election, I have absolutely no problem with that, if they show valid ID,</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. Not a fan of something, but not specified what.
+2. In favor of allowing people to register up to and including the day of the election.
+3. Approval is dependent on showing valid ID.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
         <v>48632</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>"11:04"</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>I mean, as long as we're checking the registration to something, I feel like online. Isn't that much more secure than sending in a ballot? Like yeah, you can spoof it a lot more, but one, the post office can't lose my online entry into, you know, if it's checked to, you know, that person exists, then it's more. Gives them time to look at it. Whereas, if you re making people do it in person, I really you do probably need to let them do it until election day. Because</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. Checking registration to an online system is considered more secure than sending a ballot through the mail.
+2. Online registration is less susceptible to loss compared to mail-in ballots, as the postal service cannot lose an online entry.
+3. Verification of a person's existence during online registration allows for more time to review the entry.
+4. In-person registration requires more flexibility, as people should be allowed to register until election day.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
         <v>48632</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>"11:04"</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t xml:space="preserve"> There's too many other things, it's a pain for people to go places and person especially the government that isn't open reasonable hours for people who are working.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The text mentions that there are many things that make it difficult for people.
+2. It is challenging for people to go to places, particularly for individuals working.
+3. The government is highlighted as an example of an entity that does not operate during convenient hours for working people.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
         <v>48647</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>"11:43"</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>I guess I'm not responding directly to the question except by saying I like the idea of establishing automobile, automatic voter registration because then I think that it moves away from some of the issues we're talking about in terms of registering online, for example, and with automatic voter registration, all eligible voters are eligible are able to be registered but</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The idea of automobile, automatic voter registration is favored.
+2. This method moves away from online registration issues.
+3. All eligible voters can be registered with automatic voter registration.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
         <v>48647</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>"11:43"</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t xml:space="preserve"> If people can opt out or register and more normal way.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B10" t="inlineStr">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>"12:18"</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Just to kind of take a straw poll. I'm interested. So like in the state of Montana, when you go get your driver's license down at the DMV, there's actually an additional check box. You can check that will say, hey, register to vote. I'm just interested to hear if that's another States.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
         <v>48632</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>"12:31"</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>That was actually I was about to say is Virginia does that? Which is really nice and its really good for like a lot of people but they're still going to be a population that doesn't get that which is how what I've always wanted to automatic voting. Like how do they know who was actually in the state to register them?</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B12" t="inlineStr">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>"12:48"</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>I wonder if you could do it bass like on the IRS tax returns like forced them to, you know, that that's how you know that someone lives somewhere and sorry Gina is</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
         <v>48617</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>"12:50"</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Yes. So in Massachusetts, I actually had to just renew my license today and they automatically register you, which was weird because I'm already registered voter, so they aren't they do it automatically to answer your question.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
         <v>48617</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>"12:50"</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
         <v>48647</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>"13:13"</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>I think in the booklet that we were sent it, I can't immediately find it but it said that the automatic registration they have databases that they check. The the person they check people through their databases to make sure that they're eligible to vote.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
         <v>48653</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>"13:35"</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>I'm a little embarrassed because I got my license. I mean I'm only 20, I'll be 25 soon so it's not that long ago that I got my license and I really can't remember if there was a box to check for voter registration. I think be a great way to do it. I'm a big fan of automatic enrollment for voting.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
         <v>48617</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>"13:57"</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Oh, what, I want to speak on. What I think it the online. I don't necessarily go with online voting. That's just my opinion.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker has an opinion on online voting.
+2. They do not necessarily support online voting.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
         <v>48617</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>"13:57"</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
         <v>48632</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>"14:07"</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>It's not online, voting rights just online registration online, voting would be a nightmare.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
         <v>9408</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>"14:09"</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
         <v>9408</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>"14:09"</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Yeah, I'm not really no nobody, but I think just checking you like station when you get there. I'm just old-fashioned, but that's just me.</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
         <v>48617</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>"14:23"</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Actually, no, it does. It says online. Registration will expand access to voting by register more people to vote. So maybe I misunderstood it, but it looks like it was allowing him to vote online. Also, yet I believe I could have Miss under stood, the little video, we saw</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
         <v>48617</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>"14:40"</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
         <v>48617</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>"14:41"</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B25" t="inlineStr">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>"14:43"</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>I think that's maybe later down here there. I know there's a proposal to say that and that I'm definitely you know, 100% against here is any kind of online voting but I mean, registration wise here, I could be convinced. I think what I would like to see is some kind of I'd be interested to see how they would prevent fraud, right? So maybe if you registered here and then to prove that you were really you, they sent like something in the mail to you to say, hey we notice that you're registered online. Can you like</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B26" t="inlineStr">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>"14:43"</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t xml:space="preserve"> It somehow just really more. So to, I would want to avoid people, you know, who have voter apathy, who, you know, get registered and all the sudden they're voting for for people that they would never voted for.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
         <v>48632</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>"15:25"</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>I just know, I've lived in a lot of apartments and every time we get, you know, you get a ton of people's old mail and some of the places where they have for local elections, you automatically register, we've gotten ballots, and if you're less</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
         <v>48632</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>"15:25"</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t xml:space="preserve"> You know, if you're not upstanding, it would be really tempting to check the box. I'm not a ballot and send it back, which makes me nervous because it is it's hard to keep track of everyone but at the same time you want everyone to have the opportunity.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B29" t="inlineStr">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>"15:54"</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Yeah. And by that same token here, one of the problems with you know, interior supposed to go update your license when you move. And I know when I was younger and was moving, you know, in between Apartments, I honestly didn't bother going and, you know, getting a new address on my license. So I'm sure my early years. Here I fell through the cracks right for any kind of voter registration.</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
         <v>48617</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>"16:13"</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>I guess not to hop on it. But yesterday, actually, that's the first thing. It says, allow citizens, to register to vote online. So, yes, I'm absolutely against</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker is against allowing citizens to register to vote online.
+2. The speaker's statement is in response to a proposal that was mentioned previously, but not detailed in the text.
+3. The proposal was to allow online voter registration "yesterday."
+4. The speaker's opposition is stated with certainty, using the phrase "I'm absolutely against."</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
         <v>48653</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>"16:22"</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
         <v>48653</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>"16:22"</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>I just was going to ask, how early do you have to be registered to go? I don't even know really? And then if you were saying that you had moved or whatever, right? What about people that like, have registered to vote in then they move States in between, like, what is that Gap look like, I guess.</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The user is asking about the deadline for voter registration.
+2. The user is unsure about the process for voters who have moved States.
+3. The user is inquiring about the gap in registration for voters who move States.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
         <v>48617</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>"16:44"</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>I'm it's using state-by-state. So some states allow you to give can like it's by State.</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
         <v>48617</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>"16:44"</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t xml:space="preserve"> So it depends what state you live in.</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
         <v>48647</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>"16:57"</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Yeah, it does depend on what state you you live in.</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
         <v>48653</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>"17:05"</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>How early are your guys's States, though?</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B37" t="inlineStr">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C37" t="inlineStr">
         <is>
           <t>"17:05"</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Yeah.</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B38" t="inlineStr">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C38" t="inlineStr">
         <is>
           <t>"17:05"</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t xml:space="preserve"> I was going to say for the state of Montana here. If you're willing to go and vote in person, you can vote up to the election day, you can go in there in person and vote, but a lot of people here vote by absentee ballot. I know that's what I do in order to get an absentee ballot. I think you need to register. I want to say, it's either two or three weeks before the, you know, voter day here to guarantee that you're going to get an absentee ballot in the mail.</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. In Montana, it is possible to vote in person up to the election day.
+2. Many people in Montana vote by absentee ballot.
+3. To get an absentee ballot, one probably needs to register.
+4. The deadline to register for an absentee ballot is typically two to three weeks before the election day.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
         <v>48647</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>"17:34"</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>And I was just going to add that my understanding is that there has been a Consortium of states that access one another's. Databases pertaining to voters. So that as someone moves from one state to another, they they can't, they will catch someone who hasn't bothered to to is trying to vote in both States who seems to be registered and</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. A Consortium of states exist that share voter information databases.
+2. The purpose of this is to prevent voter fraud across state lines.
+3. If a person moves from one state to another, the system can detect if they are trying to vote in both states.
+4. This system can also catch individuals who are registered in multiple states and attempting to vote in all of them.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
         <v>48647</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>"17:34"</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t xml:space="preserve"> all states and they will go. Oh, but that person moved and therefore they're not eligible and the state from which they worked.</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The text discusses the ineligibility of some individuals to vote.
+2. The reason for their ineligibility is that they have moved to a different state.
+3. These individuals will not be able to vote in the state where they previously resided.
+4. The text emphasizes that all states and the people residing in them will participate in the voting process.
+5. However, any person who has moved to a different state is no longer eligible to vote in the state they moved from.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B41" t="inlineStr">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C41" t="inlineStr">
         <is>
           <t>"18:11"</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Yeah, that the last thing to answer your other question. Alex, was how, what happens when you move States in my mind? I have the same question, I don't think there's a way to track it, because if there was like in my mind, if there was, then they could figure out, you know, if your actual ballot was cast right? Like supposedly, it's Anonymous, maybe. I know in the state of Montana when you have an absentee ballot, there's two parts to it. There's like the outer ballot where, you know, you sign your name and affidavit. So maybe they could track that and so long as they don't,</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. When someone named Alex moves States in a person's mind, they might have the same question about tracking it.
+2. The text suggests that if there was a way to track it in the person's mind, then it could be determined if a person's actual ballot was cast correctly.
+3. The text mentions that in the state of Montana, absentee ballots have two parts: an outer ballot where the person signs their name and affidavit.
+4. The text implies that it might be possible to track an absentee ballot by using the outer ballot, but it also notes that absentee ballots are supposed to be anonymous.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B42" t="inlineStr">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C42" t="inlineStr">
         <is>
           <t>"18:11"</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t xml:space="preserve"> Look on the inner ballot, which is, you know, supposedly the secret ballot, maybe they'd be able to tell and say, hey spoil it or not, if someone is voted somewhere else but I've always wondered the same thing too.</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B43" t="inlineStr">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C43" t="inlineStr">
         <is>
           <t>"20:34"</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>I've definitely got a lot of opinions on this, but I really think that any vote by mail ballots should be in before election day. And for us, personally, we go and we drop off our mail, ballots physically down at the at the County Courthouse. I don't trust the mail to deliver it on time. I know in Montana here there's been a lot of kind of noise around people that go around and collect ballots to go drop it off that. I'm kind of mixed on here, Montana's a really big state and it's really inconvenient for some people to make it to the county courthouse.</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. It is important that vote by mail ballots should be submitted before election day.
+2. The author and their family personally deliver their mail ballots to the County Courthouse.
+3. The author does not trust the mail to deliver their ballot on time.
+4. In Montana, there has been controversy around people collecting and delivering multiple ballots.
+5. The author has mixed feelings about ballot collection in Montana.
+6. Montana is a large state, and some people may find it inconvenient to go to the county courthouse.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B44" t="inlineStr">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C44" t="inlineStr">
         <is>
           <t>"20:34"</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t xml:space="preserve"> House. So I'm not as opposed to people going and collecting ballots and as far as like video monitoring at least for us in our County Courthouse because it is in the courthouse, there's actually someone that physically sits there and watches you drop in the ballot.</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
         <v>48653</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>"21:24"</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>As far as installing video cameras goes for monitoring the ballot. Who's going to be watching these video cameras? I feel like it's another step, like I want it to be protected and things, but I feel like what Ace was saying, like there's someone physically there, I feel like that's pretty good. I just don't know who's going to spend the time to watch it and I feel like that's more cost and Tech that we probably could put towards other things that might actually protect a little bit.</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B46" t="inlineStr">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C46" t="inlineStr">
         <is>
           <t>"21:50"</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>I could give you a case in point here. So and this was kind of weird here though. So the last time that we had elections, we went and dropped it off at the county courthouse and there was somebody there. So there's always the security guard their right arm security guard because it's the courthouse right. Make sure no one's going to come in and do anything. But there was I want to say it was some third party here and they actually looked at the ballots and I question if that was like legitimate for them to do but that being said it was to my advantage because they looked at and they're like hey you forgot to sign this here, you need to make sure that you sign</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The text describes an event that occurred during an election at a county courthouse.
+2. A security guard was present at the courthouse to ensure building security.
+3. A third party was also present and examining ballots.
+4. The third party noticed that a ballot lacked a signature.
+5. The lack of signature needed to be corrected for the ballot to be valid.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B47" t="inlineStr">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C47" t="inlineStr">
         <is>
           <t>"21:50"</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t xml:space="preserve"> Sign this portion, otherwise you're going to invalidate your ballot. So in that case, I was glad but I kind of wonder if you know a less scrupulous instead of individuals was there, if they'd scare people off.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
         <v>48647</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>"22:32"</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Wasn't there an incident or a series of incidents and the last election cycle where armed people would serve be standing near ballot boxes and some people said that they felt intimidated to go drop off. There are balanced. Does anybody recall that it would intimidate intimidate me if someone were standing there with a rifle who</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. There is reference to an incident or a series of incidents related to the last election cycle.
+2. Armed individuals were present near ballot boxes.
+3. Some individuals felt intimidated to drop off their ballots.
+4. The presence of people with rifles could be intimidating.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
         <v>48647</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>"22:32"</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t xml:space="preserve"> Who wasn't the security guard?</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
         <v>48632</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>"23:05"</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>I do a lot of places have all those rules, right? Like you can't protest you can't do all these things with in some you know within such a distance of the polling place that seems like that should apply to drop boxes. I don't know if it does, it's probably state-by-state again. But that seems like a safe.</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
         <v>48632</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>"23:05"</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t xml:space="preserve"> What you call it.</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
         <v>48632</v>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>"23:05"</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t xml:space="preserve"> Non non.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
         <v>48632</v>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>"23:05"</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t xml:space="preserve"> Controversial thing to at least help with that a little bit.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B54" t="inlineStr">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C54" t="inlineStr">
         <is>
           <t>"23:35"</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>I don't know, I haven't heard of anything but I wouldn't doubt it at all here, right? And I think there's, you know, even kind of like campaigning right? Like in theory they're not supposed to be able to campaign within, I think it's like 300 feet of a polling place. You're not supposed to have any political signs up, but it all comes down to hey that's what the law is on. The books is it actually enforced, who knows, right?</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The person has not heard of any issues related to campaigning near polling places.
+2. They believe that campaigning might still occur near polling places.
+3. In theory, political campaigns are not allowed to campaign within 300 feet of a polling place.
+4. The person suggests that political signs might be present near polling places.
+5. They question whether the law against campaigning near polling places is enforced.</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
         <v>48617</v>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>"23:58"</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
         <v>48617</v>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>"23:58"</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>Okay, where was I at? Oh my goodness.</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
         <v>48617</v>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>"23:58"</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t xml:space="preserve"> As far as when you said the poem, yeah, they were out Most states. Do have that and it is enforced by most likely by the other candidates. They enforce it themselves, they police it.</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
         <v>48617</v>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>"23:58"</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
         <v>48617</v>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>"23:58"</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B60" t="inlineStr">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C60" t="inlineStr">
         <is>
           <t>"25:49"</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>I'm a big fan of saying, hey, you got to show ID to vote. Now that being said, there's definitely Logistics involved with that, right? Right now. Today, I just drop my ballot off in the Box here and nobody really check. So I definitely can see how that could be costly. But to me, I don't think it's too big of a barrier. Like you're already required to show ID if you're going to, you know, buy alcohol or buy a gun or various other things. I don't think that's as much of a barrier, but I definitely recognize that it. It's going to make it a lot more complex than just simply.</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker is in favor of showing ID to vote.
+2. The speaker acknowledges logistical challenges in implementing ID requirement for voting.
+3. Currently, ID is not checked when the speaker drops off their ballot.
+4. The speaker recognizes that ID requirement could increase costs.
+5. The speaker believes that ID requirement for voting is not a significant barrier.
+6. The speaker points out that ID is already required for other activities, such as buying alcohol or guns.
+7. The speaker recognizes that ID requirement will make voting more complex.</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B61" t="inlineStr">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C61" t="inlineStr">
         <is>
           <t>"25:49"</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t xml:space="preserve"> Early dropping off your ballot.</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
         <v>48647</v>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>"26:20"</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>And I'm opposed to require requiring government-issued, photo ID and obtained. With proof of citizenship thinking about two different populations and New Mexico folks on some of the far-flung. Indian reservations Nations Pablo's, that you don't even have running water and don't have good Transportation often don't have the right, you know the up</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker is opposed to requiring government-issued, photo ID for voting.
+2. They mention two populations that might struggle with this requirement: people in some far-flung Indian reservations and people in New Mexico.
+3. Some of these reservations, like Pablo's, may not have basic amenities such as running water.
+4. Additionally, these populations may also lack good transportation.
+5. As a result, they might not have the necessary documents to obtain a photo ID.</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
         <v>48647</v>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>"26:20"</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t xml:space="preserve"> Be one person who has a driver's license but not other people and it's hard to go into the areas and get a photo ID and the second population. And Albuquerque would be homeless. Populations where people</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. You are in possession of a driver's license.
+2. Other people do not have a driver's license.
+3. It is challenging to enter certain areas and obtain a photo ID for these individuals.
+4. The second population being discussed is the homeless population in Albuquerque.
+5. This population faces difficulties in obtaining photo IDs.</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
         <v>48617</v>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="C64" t="inlineStr">
         <is>
           <t>"27:11"</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>I do agree with Heavenly uniform, haven't established, uniform, uniform, voting laws across the board, across United States, and still leave it to the States because we see what happened in Georgia when they left it to the states point taken.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker agrees with having a uniform, consistent set of voting laws.
+2. The speaker acknowledges that voting laws are not currently established uniformly across the United States.
+3. The speaker believes that voting laws should still be left to the individual States.
+4. The speaker references Georgia as an example of what can happen when voting laws are left to the States.
+5. The speaker seems to imply that the situation in Georgia supports the idea of having uniform voting laws across the country.</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
         <v>48647</v>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="C65" t="inlineStr">
         <is>
           <t>"27:36"</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>And I'm very mixed about having Congress established uniform Nationwide rules. But, you know, one of the things that occurred to me was the situation in Georgia, where Sunday, early voting was, was a lot of previously, but then taken away for some suspicious reasons.</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B66" t="inlineStr">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C66" t="inlineStr">
         <is>
           <t>"27:59"</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>Yeah, I'm mixed on that to hear II know Montana, is a really big state in there. Have been proposals to get rid of absentee or mail-in ballots, and I can tell you right now, if you did that in this state here, you would see voter turnout drop, just drastically, you know, kind of similar to what Carol mentioned. We have a lot of, you know, reservations and people that are living in really, really remote areas. So that's why I'm not. So opposed to people going and collecting ballots, right? You know, that, that was one of the complaints is like, oh, you know, people would drive down to the reservation, pick up ballots for</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B67" t="inlineStr">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C67" t="inlineStr">
         <is>
           <t>"27:59"</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t xml:space="preserve"> People and drop them off in the Box. I'm not really opposed to that but you know, it's very interesting to say that. And then in the next breath you're be like well I want voter ID. Like, how is that going to work? So there's definitely definitely something to be considered.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
         <v>48653</v>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>"28:42"</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>Do those groups that pick up the ballots for other people? Are they checking ID? Is that something that maybe some of those companies are implementing? Okay. Well I feel like that would be maybe a good place to start to if we're worried about you know marginalized populations of they could get their hands on some form of identification for these people to come and pick it up and then I am a fan of having to present idea kind of like what ASA saying if you have to have an ID for alcohol or a gun or something of that nature, I feel that it's really not asking.</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
         <v>48653</v>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>"28:42"</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t xml:space="preserve"> Being a lot to present.</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
         <v>48647</v>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>"29:15"</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>It's all for me to think about it, but I'm thinking about teenage years and fake IDs and how easy how easily the easy they were to obtain, and probably still are.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B71" t="inlineStr">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C71" t="inlineStr">
         <is>
           <t>"29:28"</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>I mean with real ID is definitely much harder but I mean even as a teen here I remember it being super easy to fake IDs. If you're very dedicated, maybe maybe a compromise that I would be definitely. Okay with is if you had some trusted, you know, if you have established some kind of web of trust, right? To say, hey, we we understand that this person is maybe going to the old folks home or it's going to these remote areas to collect ballots that. We trust that they're not, just simply dumping ballots. It's, I don't know. It's a hard and sticky,</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B72" t="inlineStr">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C72" t="inlineStr">
         <is>
           <t>"29:28"</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t xml:space="preserve"> Situation. And I can be swayed either way but we've got to do something to just avoid going out and saying, hey, you know, I'm going to give you five bucks to vote for this particular candidate. I'll make it real easy here. I'll even drop it off for you.</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
         <v>48647</v>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>"30:38"</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>I'm in favor of restoring voting rights to people who've been released from prison, they have done their time, we're saying we're restoring them to the responsibilities of the community, one of which is holding</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
         <v>48617</v>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>"30:55"</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>I agree. Also angry to restore voting rights, to those who've been incarcerated as well.</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. You agree with restoring voting rights.
+2. You are angry about the denial of voting rights to individuals who have been incarcerated.</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B75" t="inlineStr">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C75" t="inlineStr">
         <is>
           <t>"31:03"</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>On the surface, I would agree here. I would, I kind of liked it. What their proposal was though is that do it Case by case, but maybe make the default to automatically be restoring their voting rights. So for example, of someone who I would never want to see their voting rights restored to as anyone who is convicted of, you know, any kind of voter fraud or, you know, I would definitely not want to see them have their voting rights restored, but that would be such a such a marginal Corner case that I think for the, for the majority of people here, I</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B76" t="inlineStr">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C76" t="inlineStr">
         <is>
           <t>"31:03"</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t xml:space="preserve"> agree. Here is restore their rights, but put some kind of control on it.</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="n">
         <v>48653</v>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t>"31:39"</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>Yeah, I definitely agree that I think it should be a case-by-case thing. Maybe that's something that they go over at like whatever court before they get incarcerated, like well you have a possibility of getting your rights restored for</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The decision to restore civil rights of incarcerated individuals should be made on a case-by-case basis.
+2. This process might be discussed during court proceedings prior to incarceration.
+3. The topic of restoring civil rights could be covered in these court proceedings.</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B78" t="inlineStr">
+        <v>77</v>
+      </c>
+      <c r="B78" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C78" t="inlineStr">
         <is>
           <t>"31:55"</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t>I definitely think that whatever they do here that they need, if it, if it is case-by-case, there needs to be some kind of oversight to make sure that it's not just business as usual here, right? I want to stress that I would like to see a case by case, but I would say like in the 99% of the cases here, it's just restored by default unless there's like an exception for some reason.</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker believes that there should be oversight for case-by-case actions taken at the current location.
+2. The speaker emphasizes the need for a case-by-case approach.
+3. In the speaker's opinion, the default action should be restoration in 99% of the cases.
+4. The speaker allows for exceptions to the default action in certain cases.</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="n">
         <v>48632</v>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>"32:15"</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>I would agree with Carol, like, if we're trusting and, you know, think these people are ready to come back and work and live in society. Then why can't we trust them to vote? You know, that seems like it should go hand-in-hand to me.</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker agrees with Carol.
+2. They believe that if previously incarcerated individuals are considered ready to return to society and work, then they should also be trusted to vote.
+3. The speaker sees the right to vote as a logical extension of being a part of society.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="n">
         <v>48647</v>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>"32:30"</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>I'm concerned that the case by case is just one more level of Sir bureaucracy and has the capacity to fail. And I'm trying to think there was a situation in Florida, where where people have been told by some that they could vote as previous as previously in incarcerated felons and it turned out they needed to be adjudicated, but nobody, the right hand didn't know what the left was and I don't know if</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="n">
         <v>48647</v>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="C81" t="inlineStr">
         <is>
           <t>"32:30"</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t xml:space="preserve"> Buddy remembers that more clearly but it just seems to me one more can of worms so I just like to make it clear and and do it if you have been released then you can vote.</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B82" t="inlineStr">
+        <v>81</v>
+      </c>
+      <c r="B82" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C82" t="inlineStr">
         <is>
           <t>"34:36"</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>I'd be interested to understand like what currently is in place that supposedly prevents this because that was mentioned the video. It's like, well, the con is saying that this isn't needed because there's already something in place. Like I would, I would like to understand more of what's in place, how it's enforced, and has an actually ever been enforced on the surface. I really don't want to add more laws on the books because it just seems like more bureaucracy. But on the flip side here, I definitely want to make sure that</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The text is interested in understanding what currently prevents a certain situation, as mentioned in a video.
+2. It is noted that the 'con' claims that there is no need for additional measures as there are already existing safeguards.
+3. The text wants to know more about these existing measures, how they are enforced, and if they have ever been enforced in practice.
+4. There is a concern about adding more laws, as it may lead to more bureaucracy.
+5. However, there is also a desire to ensure that the situation is properly addressed.</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B83" t="inlineStr">
+        <v>82</v>
+      </c>
+      <c r="B83" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C83" t="inlineStr">
         <is>
           <t>"34:36"</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="D83" t="inlineStr">
         <is>
           <t xml:space="preserve"> That hey, if you're telling people that, hey, you can vote on the day after election and still have your vote count, like that, that kind of stuff needs to stop your, that's not cool.</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. It is not appropriate to tell people that they can vote on the day after an election and still have their vote count.
+2. This kind of information is misleading and should be stopped.
+3. Voting after the election day is not acceptable.
+4. The vote will only count if it is cast on or before the election day.</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
         <v>48647</v>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>"35:15"</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="D84" t="inlineStr">
         <is>
           <t>I guess it given the more and more concerns being expressed around elections and as more and more polarization in the country and it concerned around both fraud and intimidation. I want to be clear about that. There's accountability when people are either Miss Lee misleading or intimidating and and with a sigh would like to know a little bit more about what's already on the books.</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="n">
         <v>48617</v>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>"35:45"</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="D85" t="inlineStr">
         <is>
           <t>I'm not quite sure what they're referring to. I know here in Massachusetts, they have poll workers, which is, I was a poll worker. I have observed several elections, so I think that's where it gets to the state. When I'm I was saying earlier, I know that's previously, but this have it broadened said, leaving up to the state so but I'm not quite sure what they're referring to. The only other thing I would say is someone telling them to vote in the next day or something. I don't even know how that's possible. I don't even know how that's possible.</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="n">
         <v>9408</v>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>"36:15"</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="D86" t="inlineStr">
         <is>
           <t>I'm like what if it's not how long it's been the video did say you know it wasn't Justified whatever been used or not but it's just my opinion.</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B87" t="inlineStr">
+        <v>86</v>
+      </c>
+      <c r="B87" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C87" t="inlineStr">
         <is>
           <t>"36:39"</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>So as far as like voting the next day here, one thing that was really interesting is is like Facebook had gone out and they said in the spirit of transparency, I think was Facebook and Google did this. They showed all the types of election ads that have been bought and it was really cool. You could kind of filter down to say, okay, what was shown to this particular demographic of Voters. And it was very clear to see that I would say was definitely toting. A line of saying, you know, how you could vote right? It's like, hey, you know, you can vote by phone or you can vote by mail or are, you know, vote by</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B88" t="inlineStr">
+        <v>87</v>
+      </c>
+      <c r="B88" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C88" t="inlineStr">
         <is>
           <t>"36:39"</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t xml:space="preserve"> By the Internet, it's like that kind of stuff. Like Timmy needs to really stop and it's it's just unfair to people who aren't familiar with the system I think</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="n">
         <v>48632</v>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="C89" t="inlineStr">
         <is>
           <t>"37:23"</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t>I think the the concept is good but the enforcement would be difficult. So I'm wondering if maybe that's where they saying we already have right. Like there are libel laws and different things about advertising. I don't know, all the details, but like I'm just like, you know, you want to draw the line between people being legitimately malicious and like, someone's Crazy, Aunt who just doesn't understand something. She heard on Facebook and is repeating it. Like you do want to say that's wrong, you want to stop the misinformation but I don't think you're crazy. Aunt should get arrested.</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The user finds the concept of controlling misinformation to be good.
+2. The user believes that enforcement of such control would be difficult.
+3. The user refers to existing laws such as libel laws and advertising regulations as possible existing forms of control.
+4. The user emphasizes the need to differentiate between malicious intent and misunderstanding.
+5. The user gives an example of a misinformed person (Crazy Aunt) who shares misinformation after hearing it on Facebook.
+6. The user does not think that the Aunt should be arrested, indicating a need for a more nuanced approach to misinformation control.</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="n">
         <v>48632</v>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>"37:23"</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t xml:space="preserve"> Rested or find or something crazy. Just because they're not the brightest, you know,</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B91" t="inlineStr">
+        <v>90</v>
+      </c>
+      <c r="B91" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C91" t="inlineStr">
         <is>
           <t>"39:15"</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="D91" t="inlineStr">
         <is>
           <t>I really think that the Secretary of State still needs to be voted in. I don't like the idea of doing any kind of appointment. I would say, though, I would be in favor of having a longer term. So that way you're not subject to kind of the ups and downs of, you know, what political party is in office. I'd say maybe either a, an eight or ten year term, but by the same token, I would also like to see really strong, you know, what ability to recall them, right? So if, for example, if the Secretary of State like refuse</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The author believes that the Secretary of State should be elected through voting, not appointed.
+2. They suggest a longer term for the Secretary of State, possibly 8 or 10 years, to reduce the impact of political party changes.
+3. The author also advocates for a strong recall ability for the Secretary of State, allowing them to be removed from office if they refuse to perform their duties.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B92" t="inlineStr">
+        <v>91</v>
+      </c>
+      <c r="B92" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C92" t="inlineStr">
         <is>
           <t>"39:15"</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t xml:space="preserve"> Is has to certify election results because, you know, they don't like, who who got voted in, right? Like that, that kind of stuff needs to stop and I think you need to have them be directly accountable.</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker believes that a person or entity should be required to certify election results.
+2. The speaker suggests that this is necessary because some people or entities may not like who was voted into office and may try to interfere with the results.
+3. The speaker thinks that this kind of behavior needs to be stopped.
+4. The speaker believes that those responsible for certifying election results should be held directly accountable for their actions.</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="n">
         <v>48647</v>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>"40:00"</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
         <v>48647</v>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="C94" t="inlineStr">
         <is>
           <t>"40:00"</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
+      <c r="D94" t="inlineStr">
         <is>
           <t>Does I'm a little confused part of the one of the pros in here talking about private foundations, providing financial assistance for conducting elections. Does anybody know anything about that?</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker is expressing some confusion.
+2. They are discussing a pro mentioned in the conversation related to private foundations.
+3. The specific pro being discussed is private foundations providing financial assistance for conducting elections.
+4. The speaker is asking if anyone has any knowledge about this.</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B95" t="inlineStr">
+        <v>94</v>
+      </c>
+      <c r="B95" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C95" t="inlineStr">
         <is>
           <t>"40:17"</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="D95" t="inlineStr">
         <is>
           <t>So I don't know if you remember, I think it was was it two days? You know, to two meetings ago they were talking about the guys from Alaska, right? And they said, when they switched over to rank Choice, voting a lot of the private foundations, kind of bore the cost of doing education for that, right? They were the ones that were running the TV ad saying, this is how you vote. This is how this is, how your, you know, how you can vote on a ballot. They were the ones that were sending out the, you know, the letters to tell people to make them aware.</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B96" t="inlineStr">
+        <v>95</v>
+      </c>
+      <c r="B96" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C96" t="inlineStr">
         <is>
           <t>"40:17"</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="D96" t="inlineStr">
         <is>
           <t xml:space="preserve"> I'm personally I'm kind of split on that like I think, I think it's okay but I think there needs to be some kind of guardrail to make sure that they aren't giving bad information.</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The person is undecided about a certain topic.
+2. They think that the topic is acceptable.
+3. However, they also believe that there should be some safeguards to prevent the spreading of bad information or practices related to this topic.</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B97" t="inlineStr">
+        <v>96</v>
+      </c>
+      <c r="B97" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C97" t="inlineStr">
         <is>
           <t>"41:05"</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
+      <c r="D97" t="inlineStr">
         <is>
           <t>I mean that being said, I can see it both ways, right? Like it kind of goes back to an earlier discussion, we had right. Is this like Civics really needs to be taught some how in a fair way in the in the public education system because you have to give everyone at least some kind of base level, understanding of how the system works. It's super unfair to necessarily like depend on either Private Industry or even you know the populace themself to inform themselves because</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B98" t="inlineStr">
+        <v>97</v>
+      </c>
+      <c r="B98" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C98" t="inlineStr">
         <is>
           <t>"41:05"</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="D98" t="inlineStr">
         <is>
           <t xml:space="preserve"> They're not always going to do it. Unfortunately.</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="n">
         <v>48632</v>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="C99" t="inlineStr">
         <is>
           <t>"46:22"</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
+      <c r="D99" t="inlineStr">
         <is>
           <t>Could we combine Ace and Carol's question a little bit. So we make sure to get both of them like, you know, prevent election, interference and intimidation just a thought, not that, they seem to answer questions anyways, but,</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. It is suggested to combine Ace and Carol's questions to ensure both of their perspectives are addressed.
+2. The goal is to prevent election interference and intimidation.
+3. It is noted that Ace and Carol generally answer questions when asked.</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="n">
         <v>48647</v>
       </c>
-      <c r="B100" t="inlineStr">
+      <c r="C100" t="inlineStr">
         <is>
           <t>"46:37"</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="D100" t="inlineStr">
         <is>
           <t>That's that'd be fine with me because I think he's Aces question is a slightly broader one than mine and I was going to suggest withdrawing mine but I think that's a good suggestion to capture the intimidation aspect.</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The speaker is fine with a certain suggestion.
+2. The speaker initially considered withdrawing their question.
+3. The speaker thinks the question proposed is a good one.
+4. The question proposed relates to the aspect of intimidation.</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="n">
         <v>48653</v>
       </c>
-      <c r="B101" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>"46:51"</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="D101" t="inlineStr">
         <is>
           <t>I also think you should add not just laws but I like Carol's idea of penalties laws and penalties.</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1. The reader thinks it is a good idea to add not just laws but also penalties to the system.
+2. This suggestion is similar to an earlier idea from Carol.</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>9648</v>
-      </c>
-      <c r="B102" t="inlineStr">
+        <v>101</v>
+      </c>
+      <c r="B102" t="n">
+        <v>9648</v>
+      </c>
+      <c r="C102" t="inlineStr">
         <is>
           <t>"46:58"</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
+      <c r="D102" t="inlineStr">
         <is>
           <t>Yeah. And I mean, kind of same way I just wanted to say that even though we might not be able to get our questions answered that, they will take these and take them to the, The Next Step here, whenever they producer documents to give to policymakers, they're going to kind of combine a lot of these. So stronger laws these</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="n">
         <v>48647</v>
       </c>
-      <c r="B103" t="inlineStr">
+      <c r="C103" t="inlineStr">
         <is>
           <t>"47:35"</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="D103" t="inlineStr">
         <is>
           <t>We say constitutional instead of Constitution.</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="n">
         <v>48632</v>
       </c>
-      <c r="B104" t="inlineStr">
+      <c r="C104" t="inlineStr">
         <is>
           <t>"47:39"</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="D104" t="inlineStr">
         <is>
           <t>I wondered if that was wrong grammatically.</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="n">
         <v>48647</v>
       </c>
-      <c r="B105" t="inlineStr">
+      <c r="C105" t="inlineStr">
         <is>
           <t>"48:12"</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr">
+      <c r="D105" t="inlineStr">
         <is>
           <t>I'm fine. It delete again since we've really captured it in Aces question.</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="n">
         <v>48632</v>
       </c>
-      <c r="B106" t="inlineStr">
+      <c r="C106" t="inlineStr">
         <is>
           <t>"48:19"</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr">
+      <c r="D106" t="inlineStr">
         <is>
           <t>like, I mean leave it on there because then they'll know we thought about it twice but</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>

</xml_diff>